<commit_message>
Modificaciones adicionales informe previo II
</commit_message>
<xml_diff>
--- a/2. MODELO MATEMATICO 2DO ORDEN/INFORME PREVIO/calculo_rc.xlsx
+++ b/2. MODELO MATEMATICO 2DO ORDEN/INFORME PREVIO/calculo_rc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNSAAC\SEMESTRE VIII\lab-control-i\2. MODELO MATEMATICO 2DO ORDEN\INFORME PREVIO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bremdows\UNSAAC\SEMESTRE VIII\lab-control-i\2. MODELO MATEMATICO 2DO ORDEN\INFORME PREVIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32F993D-C806-443F-BCD5-EF7CF89A012D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81085907-8D7A-48E7-8D19-DEB63297AAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="13935" windowHeight="16200" xr2:uid="{FE5A758F-3994-4092-854E-C1DBB8CE080E}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="11520" windowHeight="12504" xr2:uid="{FE5A758F-3994-4092-854E-C1DBB8CE080E}"/>
   </bookViews>
   <sheets>
     <sheet name="Implementación" sheetId="1" r:id="rId1"/>
@@ -149,10 +149,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -472,17 +471,17 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -510,7 +509,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -530,7 +529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>$B$1^2*4*B3/(9)</f>
         <v>1.3675213675213676E-6</v>
@@ -540,11 +539,11 @@
         <v>9.9999999999999991E-6</v>
       </c>
       <c r="C3">
-        <f>3/(2*$D$1*B3)</f>
+        <f t="shared" ref="C3:C9" si="0">3/(2*$D$1*B3)</f>
         <v>7500.0000000000009</v>
       </c>
       <c r="F3">
-        <f>($G$1^2*4*G3)/9</f>
+        <f t="shared" ref="F3:F10" si="1">($G$1^2*4*G3)/9</f>
         <v>4.4469653998865575E-6</v>
       </c>
       <c r="G3">
@@ -556,7 +555,7 @@
         <v>3571.4285714285716</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>$B$1^2*4*B4/(9)</f>
         <v>6.427350427350428E-6</v>
@@ -566,11 +565,11 @@
         <v>4.6999999999999997E-5</v>
       </c>
       <c r="C4">
-        <f>3/(2*$D$1*B4)</f>
+        <f t="shared" si="0"/>
         <v>1595.7446808510638</v>
       </c>
       <c r="F4">
-        <f>($G$1^2*4*G4)/9</f>
+        <f t="shared" si="1"/>
         <v>2.0900737379466819E-5</v>
       </c>
       <c r="G4">
@@ -578,11 +577,11 @@
         <v>4.6999999999999997E-5</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H11" si="0">3/(2*$I$1*G4)</f>
+        <f t="shared" ref="H4:H11" si="2">3/(2*$I$1*G4)</f>
         <v>759.87841945288756</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>$B$1^2*4*B5/(9)</f>
         <v>1.3675213675213674E-5</v>
@@ -592,11 +591,11 @@
         <v>9.9999999999999991E-5</v>
       </c>
       <c r="C5">
-        <f>3/(2*$D$1*B5)</f>
+        <f t="shared" si="0"/>
         <v>750</v>
       </c>
       <c r="F5">
-        <f>($G$1^2*4*G5)/9</f>
+        <f t="shared" si="1"/>
         <v>4.4469653998865572E-5</v>
       </c>
       <c r="G5">
@@ -604,13 +603,13 @@
         <v>9.9999999999999991E-5</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>357.14285714285717</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" ref="A6:A15" si="1">$B$1^2*4*B6/(9)</f>
+        <f t="shared" ref="A6:A15" si="3">$B$1^2*4*B6/(9)</f>
         <v>6.4273504273504274E-5</v>
       </c>
       <c r="B6">
@@ -618,11 +617,11 @@
         <v>4.6999999999999999E-4</v>
       </c>
       <c r="C6">
-        <f>3/(2*$D$1*B6)</f>
+        <f t="shared" si="0"/>
         <v>159.57446808510639</v>
       </c>
       <c r="F6">
-        <f>($G$1^2*4*G6)/9</f>
+        <f t="shared" si="1"/>
         <v>2.0900737379466822E-4</v>
       </c>
       <c r="G6">
@@ -630,13 +629,13 @@
         <v>4.6999999999999999E-4</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>75.98784194528875</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.3675213675213676E-4</v>
       </c>
       <c r="B7">
@@ -644,11 +643,11 @@
         <v>1E-3</v>
       </c>
       <c r="C7">
-        <f>3/(2*$D$1*B7)</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="F7">
-        <f>($G$1^2*4*G7)/9</f>
+        <f t="shared" si="1"/>
         <v>4.4469653998865575E-4</v>
       </c>
       <c r="G7">
@@ -656,13 +655,13 @@
         <v>1E-3</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>35.714285714285715</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.0085470085470087E-6</v>
       </c>
       <c r="B8">
@@ -670,11 +669,11 @@
         <v>2.1999999999999999E-5</v>
       </c>
       <c r="C8">
-        <f>3/(2*$D$1*B8)</f>
+        <f t="shared" si="0"/>
         <v>3409.0909090909095</v>
       </c>
       <c r="F8">
-        <f>($G$1^2*4*G8)/9</f>
+        <f t="shared" si="1"/>
         <v>9.7833238797504279E-6</v>
       </c>
       <c r="G8">
@@ -682,25 +681,25 @@
         <v>2.1999999999999999E-5</v>
       </c>
       <c r="H8">
+        <f t="shared" si="2"/>
+        <v>1623.3766233766235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="3"/>
+        <v>1.3675213675213676E-4</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ref="B9:B15" si="4">1000*10^-6</f>
+        <v>1E-3</v>
+      </c>
+      <c r="C9">
         <f t="shared" si="0"/>
-        <v>1623.3766233766235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="1"/>
-        <v>1.3675213675213676E-4</v>
-      </c>
-      <c r="B9">
-        <f t="shared" ref="B7:B15" si="2">1000*10^-6</f>
-        <v>1E-3</v>
-      </c>
-      <c r="C9">
-        <f>3/(2*$D$1*B9)</f>
         <v>75</v>
       </c>
       <c r="F9">
-        <f>($G$1^2*4*G9)/9</f>
+        <f t="shared" si="1"/>
         <v>2.0900737379466822E-6</v>
       </c>
       <c r="G9">
@@ -708,110 +707,110 @@
         <v>4.6999999999999999E-6</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7598.7841945288756</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.3675213675213676E-4</v>
       </c>
       <c r="B10">
+        <f t="shared" si="4"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:C15" si="5">3/(2*$D$1*B10)</f>
+        <v>75</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" t="e">
         <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="3"/>
+        <v>1.3675213675213676E-4</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="4"/>
         <v>1E-3</v>
       </c>
-      <c r="C10">
-        <f t="shared" ref="C4:C15" si="3">3/(2*$D$1*B10)</f>
+      <c r="C11">
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
-      <c r="F10">
-        <f>($G$1^2*4*G10)/9</f>
-        <v>0</v>
-      </c>
-      <c r="H10" t="e">
-        <f t="shared" si="0"/>
+      <c r="H11" t="e">
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="1"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="3"/>
         <v>1.3675213675213676E-4</v>
       </c>
-      <c r="B11">
-        <f t="shared" si="2"/>
+      <c r="B12">
+        <f t="shared" si="4"/>
         <v>1E-3</v>
       </c>
-      <c r="C11">
-        <f t="shared" si="3"/>
+      <c r="C12">
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
-      <c r="H11" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="3"/>
         <v>1.3675213675213676E-4</v>
       </c>
-      <c r="B12">
-        <f t="shared" si="2"/>
+      <c r="B13">
+        <f t="shared" si="4"/>
         <v>1E-3</v>
       </c>
-      <c r="C12">
-        <f t="shared" si="3"/>
+      <c r="C13">
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="1"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="3"/>
         <v>1.3675213675213676E-4</v>
       </c>
-      <c r="B13">
-        <f t="shared" si="2"/>
+      <c r="B14">
+        <f t="shared" si="4"/>
         <v>1E-3</v>
       </c>
-      <c r="C13">
-        <f t="shared" si="3"/>
+      <c r="C14">
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="1"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="3"/>
         <v>1.3675213675213676E-4</v>
       </c>
-      <c r="B14">
-        <f t="shared" si="2"/>
+      <c r="B15">
+        <f t="shared" si="4"/>
         <v>1E-3</v>
       </c>
-      <c r="C14">
-        <f t="shared" si="3"/>
+      <c r="C15">
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="1"/>
-        <v>1.3675213675213676E-4</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="2"/>
-        <v>1E-3</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="3"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -825,7 +824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>325</v>
       </c>
@@ -841,7 +840,7 @@
         <v>20.994046775217015</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
@@ -849,7 +848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22">
         <f>D1/(2*B20)</f>
         <v>0.55470019622522915</v>
@@ -859,7 +858,7 @@
         <v>1.000283567282036</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F24" s="1" t="s">
         <v>13</v>
       </c>
@@ -867,7 +866,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F25">
         <f>(2*G22)/G20</f>
         <v>9.5292115711854808E-2</v>
@@ -877,7 +876,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
@@ -885,7 +884,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
@@ -893,7 +892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>325</v>
       </c>
@@ -902,18 +901,18 @@
         <v>18.027756377319946</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30">
         <f>D1/(2*B28)</f>
         <v>0.55470019622522915</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -921,17 +920,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <f>PI()/(B32)</f>
         <v>0.20943951023931953</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="3">
         <f>B28*SQRT(1-B30^2)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>13</v>
       </c>
@@ -939,7 +938,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <f>4/(B30*B28)</f>
         <v>0.4</v>
@@ -949,12 +948,12 @@
         <v>9.9846035320541246E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <f>B28*B30</f>
         <v>10</v>
@@ -970,16 +969,16 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -996,7 +995,7 @@
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1">
         <f>I20</f>
         <v>1.0564771737160452</v>
       </c>
@@ -1007,7 +1006,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1027,7 +1026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>$B$1^2*4*B3/(9)</f>
         <v>6.8376068376068386E-8</v>
@@ -1041,7 +1040,7 @@
         <v>75000</v>
       </c>
       <c r="G3">
-        <f>($H$1^2*4*H3)/9</f>
+        <f t="shared" ref="G3:G10" si="0">($H$1^2*4*H3)/9</f>
         <v>4.9606400825913001E-6</v>
       </c>
       <c r="H3">
@@ -1053,7 +1052,7 @@
         <v>4838.709677419356</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>$B$1^2*4*B4/(9)</f>
         <v>6.8376068376068378E-7</v>
@@ -1063,11 +1062,11 @@
         <v>9.9999999999999991E-5</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C15" si="0">3/(2*$D$1*B4)</f>
+        <f t="shared" ref="C4:C15" si="1">3/(2*$D$1*B4)</f>
         <v>7500.0000000000009</v>
       </c>
       <c r="G4">
-        <f>($H$1^2*4*H4)/9</f>
+        <f t="shared" si="0"/>
         <v>4.9606400825913007E-5</v>
       </c>
       <c r="H4">
@@ -1075,11 +1074,11 @@
         <v>9.9999999999999991E-5</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I11" si="1">3/(2*$J$1*H4)</f>
+        <f t="shared" ref="I4:I11" si="2">3/(2*$J$1*H4)</f>
         <v>483.87096774193549</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>$B$1^2*4*B5/(9)</f>
         <v>3.213675213675214E-6</v>
@@ -1089,11 +1088,11 @@
         <v>4.6999999999999999E-4</v>
       </c>
       <c r="C5">
+        <f t="shared" si="1"/>
+        <v>1595.7446808510638</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="0"/>
-        <v>1595.7446808510638</v>
-      </c>
-      <c r="G5">
-        <f>($H$1^2*4*H5)/9</f>
         <v>2.3315008388179114E-4</v>
       </c>
       <c r="H5">
@@ -1101,13 +1100,13 @@
         <v>4.6999999999999999E-4</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>102.95126973232671</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" ref="A6:A15" si="2">$B$1^2*4*B6/(9)</f>
+        <f t="shared" ref="A6:A15" si="3">$B$1^2*4*B6/(9)</f>
         <v>6.8376068376068387E-6</v>
       </c>
       <c r="B6">
@@ -1115,11 +1114,11 @@
         <v>1E-3</v>
       </c>
       <c r="C6">
+        <f t="shared" si="1"/>
+        <v>750</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="0"/>
-        <v>750</v>
-      </c>
-      <c r="G6">
-        <f>($H$1^2*4*H6)/9</f>
         <v>4.9606400825913009E-4</v>
       </c>
       <c r="H6">
@@ -1127,13 +1126,13 @@
         <v>1E-3</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48.387096774193552</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5042735042735044E-7</v>
       </c>
       <c r="B7">
@@ -1141,11 +1140,11 @@
         <v>2.1999999999999999E-5</v>
       </c>
       <c r="C7">
+        <f t="shared" si="1"/>
+        <v>34090.909090909088</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="0"/>
-        <v>34090.909090909088</v>
-      </c>
-      <c r="G7">
-        <f>($H$1^2*4*H7)/9</f>
         <v>1.0913408181700861E-5</v>
       </c>
       <c r="H7">
@@ -1153,13 +1152,13 @@
         <v>2.1999999999999999E-5</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2199.4134897360705</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.2136752136752138E-7</v>
       </c>
       <c r="B8">
@@ -1167,109 +1166,109 @@
         <v>4.6999999999999997E-5</v>
       </c>
       <c r="C8">
+        <f t="shared" si="1"/>
+        <v>15957.44680851064</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="0"/>
-        <v>15957.44680851064</v>
-      </c>
-      <c r="G8">
-        <f>($H$1^2*4*H8)/9</f>
         <v>0</v>
       </c>
       <c r="I8" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C9" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" t="e">
         <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="C9" t="e">
+      <c r="C10" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" t="e">
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G9">
-        <f>($H$1^2*4*H9)/9</f>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I9" t="e">
+      <c r="C11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="I11" t="e">
         <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="C10" t="e">
-        <f t="shared" si="0"/>
+      <c r="C12" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G10">
-        <f>($H$1^2*4*H10)/9</f>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I10" t="e">
+      <c r="C13" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="2"/>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="C11" t="e">
-        <f t="shared" si="0"/>
+      <c r="C14" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I11" t="e">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C15" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C12" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C14" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C15" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1280,7 +1279,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -1300,7 +1299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>65</v>
       </c>
@@ -1324,7 +1323,7 @@
         <v>1.0564771737160452</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1344,7 +1343,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <f>B20*SQRT(1-C20^2)</f>
         <v>7.9999999999999991</v>
@@ -1370,7 +1369,7 @@
         <v>15.499999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
@@ -1384,7 +1383,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <f>4/(C20*B20)</f>
         <v>4</v>

</xml_diff>

<commit_message>
Funcion de transferencia y Toolbox de MATLAB
</commit_message>
<xml_diff>
--- a/2. MODELO MATEMATICO 2DO ORDEN/INFORME PREVIO/calculo_rc.xlsx
+++ b/2. MODELO MATEMATICO 2DO ORDEN/INFORME PREVIO/calculo_rc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bremdows\UNSAAC\SEMESTRE VIII\lab-control-i\2. MODELO MATEMATICO 2DO ORDEN\INFORME PREVIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81085907-8D7A-48E7-8D19-DEB63297AAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A72218-4694-47B0-801D-498D2BC52A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="11520" windowHeight="12504" xr2:uid="{FE5A758F-3994-4092-854E-C1DBB8CE080E}"/>
+    <workbookView xWindow="11520" yWindow="456" windowWidth="11520" windowHeight="12504" xr2:uid="{FE5A758F-3994-4092-854E-C1DBB8CE080E}"/>
   </bookViews>
   <sheets>
     <sheet name="Implementación" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="22">
   <si>
     <t>R</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Atenu</t>
+  </si>
+  <si>
+    <t>Te</t>
   </si>
 </sst>
 </file>
@@ -471,7 +474,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -883,6 +886,9 @@
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F26" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -890,6 +896,10 @@
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="F27">
+        <f>F25*4</f>
+        <v>0.38116846284741923</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -969,7 +979,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Avance con el sistema Sobre Amortiguado
</commit_message>
<xml_diff>
--- a/2. MODELO MATEMATICO 2DO ORDEN/INFORME PREVIO/calculo_rc.xlsx
+++ b/2. MODELO MATEMATICO 2DO ORDEN/INFORME PREVIO/calculo_rc.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bremdows\UNSAAC\SEMESTRE VIII\lab-control-i\2. MODELO MATEMATICO 2DO ORDEN\INFORME PREVIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A72218-4694-47B0-801D-498D2BC52A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4363FFB-74E0-4C23-8DFE-B19194E84AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="456" windowWidth="11520" windowHeight="12504" xr2:uid="{FE5A758F-3994-4092-854E-C1DBB8CE080E}"/>
   </bookViews>
   <sheets>
     <sheet name="Implementación" sheetId="1" r:id="rId1"/>
     <sheet name="Polos Bremdow" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="22">
   <si>
     <t>R</t>
   </si>
@@ -474,7 +475,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,8 +543,8 @@
         <v>9.9999999999999991E-6</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C9" si="0">3/(2*$D$1*B3)</f>
-        <v>7500.0000000000009</v>
+        <f t="shared" ref="C3:C4" si="0">3/($D$1*B3)</f>
+        <v>15000.000000000002</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F10" si="1">($G$1^2*4*G3)/9</f>
@@ -569,7 +570,7 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>1595.7446808510638</v>
+        <v>3191.4893617021276</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
@@ -594,8 +595,8 @@
         <v>9.9999999999999991E-5</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>750</v>
+        <f>3/($D$1*B5)</f>
+        <v>1500</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
@@ -620,8 +621,8 @@
         <v>4.6999999999999999E-4</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>159.57446808510639</v>
+        <f t="shared" ref="C6:C15" si="4">3/($D$1*B6)</f>
+        <v>319.14893617021278</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
@@ -646,8 +647,8 @@
         <v>1E-3</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>75</v>
+        <f t="shared" si="4"/>
+        <v>150</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
@@ -672,8 +673,8 @@
         <v>2.1999999999999999E-5</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>3409.0909090909095</v>
+        <f t="shared" si="4"/>
+        <v>6818.1818181818189</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
@@ -691,15 +692,15 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="3"/>
-        <v>1.3675213675213676E-4</v>
+        <v>1.3675213675213676E-6</v>
       </c>
       <c r="B9">
-        <f t="shared" ref="B9:B15" si="4">1000*10^-6</f>
-        <v>1E-3</v>
+        <f>10*10^-6</f>
+        <v>9.9999999999999991E-6</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>75</v>
+        <f t="shared" si="4"/>
+        <v>15000.000000000002</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
@@ -720,12 +721,12 @@
         <v>1.3675213675213676E-4</v>
       </c>
       <c r="B10">
+        <f t="shared" ref="B9:B15" si="5">1000*10^-6</f>
+        <v>1E-3</v>
+      </c>
+      <c r="C10">
         <f t="shared" si="4"/>
-        <v>1E-3</v>
-      </c>
-      <c r="C10">
-        <f t="shared" ref="C10:C15" si="5">3/(2*$D$1*B10)</f>
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
@@ -742,12 +743,12 @@
         <v>1.3675213675213676E-4</v>
       </c>
       <c r="B11">
+        <f t="shared" si="5"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C11">
         <f t="shared" si="4"/>
-        <v>1E-3</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="5"/>
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="H11" t="e">
         <f t="shared" si="2"/>
@@ -760,12 +761,12 @@
         <v>1.3675213675213676E-4</v>
       </c>
       <c r="B12">
+        <f t="shared" si="5"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C12">
         <f t="shared" si="4"/>
-        <v>1E-3</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="5"/>
-        <v>75</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -774,12 +775,12 @@
         <v>1.3675213675213676E-4</v>
       </c>
       <c r="B13">
+        <f t="shared" si="5"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
         <f t="shared" si="4"/>
-        <v>1E-3</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="5"/>
-        <v>75</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -788,12 +789,12 @@
         <v>1.3675213675213676E-4</v>
       </c>
       <c r="B14">
+        <f t="shared" si="5"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C14">
         <f t="shared" si="4"/>
-        <v>1E-3</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="5"/>
-        <v>75</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -802,12 +803,12 @@
         <v>1.3675213675213676E-4</v>
       </c>
       <c r="B15">
+        <f t="shared" si="5"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C15">
         <f t="shared" si="4"/>
-        <v>1E-3</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="5"/>
-        <v>75</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -979,7 +980,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1414,4 +1415,341 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC798210-21BD-4E89-84CF-93BB2956A098}">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1">
+        <f>B22</f>
+        <v>0.44721359549995793</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>$B$1^2*4*B3/(9)</f>
+        <v>8.8888888888888866E-7</v>
+      </c>
+      <c r="B3">
+        <f>10*10^-6</f>
+        <v>9.9999999999999991E-6</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C15" si="0">3/(2*$D$1*B3)</f>
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>$B$1^2*4*B4/(9)</f>
+        <v>4.1777777777777772E-6</v>
+      </c>
+      <c r="B4">
+        <f>47*10^-6</f>
+        <v>4.6999999999999997E-5</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>15957.44680851064</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f>$B$1^2*4*B5/(9)</f>
+        <v>8.8888888888888883E-6</v>
+      </c>
+      <c r="B5">
+        <f>100*10^-6</f>
+        <v>9.9999999999999991E-5</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>7500.0000000000009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" ref="A6:A15" si="1">$B$1^2*4*B6/(9)</f>
+        <v>4.1777777777777774E-5</v>
+      </c>
+      <c r="B6">
+        <f>470*10^-6</f>
+        <v>4.6999999999999999E-4</v>
+      </c>
+      <c r="C6">
+        <f>3/(2*$D$1*B6)</f>
+        <v>1595.7446808510638</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>8.888888888888888E-5</v>
+      </c>
+      <c r="B7">
+        <f>1000*10^-6</f>
+        <v>1E-3</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>1.9555555555555551E-6</v>
+      </c>
+      <c r="B8">
+        <f>22*10^-6</f>
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>34090.909090909088</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>8.888888888888888E-5</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ref="B9:B15" si="2">1000*10^-6</f>
+        <v>1E-3</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>8.888888888888888E-5</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="2"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>8.888888888888888E-5</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="2"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>8.888888888888888E-5</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="2"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>8.888888888888888E-5</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="2"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>8.888888888888888E-5</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="2"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>8.888888888888888E-5</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="2"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <f>SQRT(A20)</f>
+        <v>2.2360679774997898</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <f>D1/(2*B20)</f>
+        <v>0.44721359549995793</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>325</v>
+      </c>
+      <c r="B28">
+        <f>SQRT(A28)</f>
+        <v>18.027756377319946</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <f>D1/(2*B28)</f>
+        <v>5.5470019622522911E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f>PI()/(B32)</f>
+        <v>0.17453292519943295</v>
+      </c>
+      <c r="B32" s="3">
+        <f>B28*SQRT(1-B30^2)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f>4/(B30*B28)</f>
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <f>1.8/(B28)</f>
+        <v>9.9846035320541246E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f>B28*B30</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>